<commit_message>
Tests añadidos: Login_CLU_OK Login_CLU_KO Consulta_Bola_Facturas Consulta_CPs Consulta_Datos_Contrato
</commit_message>
<xml_diff>
--- a/miOrangeApp/testcases.xlsx
+++ b/miOrangeApp/testcases.xlsx
@@ -4,14 +4,15 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22152" windowHeight="7836" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCLU_Test_Cases_OK" sheetId="1" r:id="rId1"/>
     <sheet name="LoginCLU_Test_Cases_KO" sheetId="2" r:id="rId2"/>
     <sheet name="Consultas_Test_Cases_OK" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:L25"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="10">
   <si>
     <t>zxcvbnm,</t>
   </si>
@@ -47,22 +48,10 @@
     <t>Contraseña Vacia</t>
   </si>
   <si>
-    <t>E86713328</t>
-  </si>
-  <si>
     <t>Login con Msisdn OK, Password OK. Recurso Residencial Pospago No Love</t>
   </si>
   <si>
-    <t>Login CIF OK, Password OK, Recurso empresa Pospago Love</t>
-  </si>
-  <si>
     <t>Recurso Residencial Pospago. Acceso Dashboard OK.</t>
-  </si>
-  <si>
-    <t>635656921</t>
-  </si>
-  <si>
-    <t>44332211</t>
   </si>
 </sst>
 </file>
@@ -180,7 +169,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -192,7 +181,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -200,8 +188,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -489,7 +475,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A4" sqref="A4:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -519,57 +505,15 @@
         <v>4</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="22">
-        <v>44332211</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="5">
-        <v>13071971</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>10</v>
-      </c>
-    </row>
+    <row r="4" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -600,7 +544,7 @@
       <c r="A2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="17" t="s">
         <v>0</v>
       </c>
     </row>
@@ -613,24 +557,24 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="13">
+      <c r="B4" s="12">
         <v>655758100</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="15"/>
+      <c r="B5" s="14"/>
     </row>
     <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="16" t="s">
         <v>7</v>
       </c>
     </row>
@@ -638,7 +582,7 @@
       <c r="A7" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="18">
+      <c r="B7" s="17">
         <v>655758200</v>
       </c>
     </row>
@@ -646,7 +590,7 @@
       <c r="A8" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="17" t="s">
         <v>0</v>
       </c>
     </row>
@@ -654,31 +598,31 @@
       <c r="A9" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="17" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="13">
+      <c r="B10" s="12">
         <v>655758100</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="15">
+      <c r="B11" s="14">
         <v>123456</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="16" t="s">
         <v>5</v>
       </c>
     </row>
@@ -689,10 +633,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -701,55 +645,38 @@
     <col min="2" max="2" width="61.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="20" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="19" t="s">
+      <c r="B1" s="18">
+        <v>655758100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="20" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="11" t="s">
+      <c r="B2" s="19" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="21">
-        <v>655758100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="24" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="22" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>11</v>
-      </c>
+      <c r="B3" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Subida Excel con los datos para los testcases
</commit_message>
<xml_diff>
--- a/miOrangeApp/testcases.xlsx
+++ b/miOrangeApp/testcases.xlsx
@@ -635,8 +635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -672,9 +672,13 @@
     <row r="4" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B13" s="1"/>
-    </row>
+    <row r="7" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Toggle para activar o desactivar la captura de evidencias.
</commit_message>
<xml_diff>
--- a/miOrangeApp/testcases.xlsx
+++ b/miOrangeApp/testcases.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="15">
   <si>
     <t>zxcvbnm,</t>
   </si>
@@ -48,10 +48,25 @@
     <t>Contraseña Vacia</t>
   </si>
   <si>
-    <t>Login con Msisdn OK, Password OK. Recurso Residencial Pospago No Love</t>
-  </si>
-  <si>
-    <t>Recurso Residencial Pospago. Acceso Dashboard OK.</t>
+    <t>Recurso Residencial Pospago. Acceso Dashboard OK.Sin CPs</t>
+  </si>
+  <si>
+    <t>Recurso Residencial Pospago. Acceso Dashboard OK.Con CP en Tarifa</t>
+  </si>
+  <si>
+    <t>E86713328</t>
+  </si>
+  <si>
+    <t>13071971</t>
+  </si>
+  <si>
+    <t>Recurso Prepago. Login_CLU por MSISDN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recurso Residencial Pospago NoLove. Login_CLU por MSISDN. </t>
+  </si>
+  <si>
+    <t>Recurso Empresa Pospago Love. Login_CLU por CIF.</t>
   </si>
 </sst>
 </file>
@@ -75,7 +90,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -94,6 +109,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="7">
     <border>
@@ -169,7 +190,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -192,6 +213,10 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -475,7 +500,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD9"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -505,15 +530,57 @@
         <v>4</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="3">
+        <v>615761875</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="5">
+        <v>11223344</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -525,7 +592,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -636,7 +703,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD18"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -666,12 +733,33 @@
         <v>4</v>
       </c>
       <c r="B3" s="16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3">
+        <v>635656921</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="5">
+        <v>44332211</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Actualizacion Excel de Recursos y toggle captura evidencias a false
</commit_message>
<xml_diff>
--- a/miOrangeApp/testcases.xlsx
+++ b/miOrangeApp/testcases.xlsx
@@ -4,15 +4,16 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22152" windowHeight="7836" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10416" windowHeight="7344" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCLU_Test_Cases_OK" sheetId="1" r:id="rId1"/>
     <sheet name="LoginCLU_Test_Cases_KO" sheetId="2" r:id="rId2"/>
     <sheet name="Consultas_Test_Cases_OK" sheetId="4" r:id="rId3"/>
+    <sheet name="Recursos" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:L25"/>
+  <oleSize ref="A1:M25"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="21">
   <si>
     <t>zxcvbnm,</t>
   </si>
@@ -67,6 +68,24 @@
   </si>
   <si>
     <t>Recurso Empresa Pospago Love. Login_CLU por CIF.</t>
+  </si>
+  <si>
+    <t>Residencial Pospago NoLove</t>
+  </si>
+  <si>
+    <t>Residencial Pospago Love</t>
+  </si>
+  <si>
+    <t>Empresa Pospago Love</t>
+  </si>
+  <si>
+    <t>Prepago</t>
+  </si>
+  <si>
+    <t>beta1234</t>
+  </si>
+  <si>
+    <t>43515511V</t>
   </si>
 </sst>
 </file>
@@ -190,7 +209,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -217,6 +236,7 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -500,7 +520,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -702,8 +722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -771,4 +791,275 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3">
+        <v>615761875</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="5">
+        <v>11223344</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="23">
+        <v>655758100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="3">
+        <v>635656921</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="5">
+        <v>44332211</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="23">
+        <v>691852789</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="24">
+        <v>4603026</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="3">
+        <v>653318896</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="5">
+        <v>87654321</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="23">
+        <v>635658486</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="25" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="3">
+        <v>635658400</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" s="5">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="24">
+        <v>37560000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="25" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="23">
+        <v>635649220</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B29" s="24">
+        <v>44332211</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" s="25" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="33" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="34" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="35" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="37" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="41" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Subidos nuevos casos de pruebas:
</commit_message>
<xml_diff>
--- a/miOrangeApp/testcases.xlsx
+++ b/miOrangeApp/testcases.xlsx
@@ -4,16 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10416" windowHeight="7344" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22152" windowHeight="7836" tabRatio="899"/>
   </bookViews>
   <sheets>
-    <sheet name="LoginCLU_Test_Cases_OK" sheetId="1" r:id="rId1"/>
-    <sheet name="LoginCLU_Test_Cases_KO" sheetId="2" r:id="rId2"/>
-    <sheet name="Consultas_Test_Cases_OK" sheetId="4" r:id="rId3"/>
-    <sheet name="Recursos" sheetId="5" r:id="rId4"/>
+    <sheet name="LoginCLU_Tests_OK" sheetId="1" r:id="rId1"/>
+    <sheet name="LoginCLU_Tests_KO" sheetId="2" r:id="rId2"/>
+    <sheet name="Consulta_CPs" sheetId="4" r:id="rId3"/>
+    <sheet name="Consulta_Contrato" sheetId="7" r:id="rId4"/>
+    <sheet name="Consulta_Factura" sheetId="8" r:id="rId5"/>
+    <sheet name="Consulta_MiLinea" sheetId="6" r:id="rId6"/>
+    <sheet name="Recursos" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:M25"/>
+  <oleSize ref="A1:O25"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="27">
   <si>
     <t>zxcvbnm,</t>
   </si>
@@ -49,43 +52,61 @@
     <t>Contraseña Vacia</t>
   </si>
   <si>
-    <t>Recurso Residencial Pospago. Acceso Dashboard OK.Sin CPs</t>
-  </si>
-  <si>
-    <t>Recurso Residencial Pospago. Acceso Dashboard OK.Con CP en Tarifa</t>
-  </si>
-  <si>
     <t>E86713328</t>
   </si>
   <si>
     <t>13071971</t>
   </si>
   <si>
-    <t>Recurso Prepago. Login_CLU por MSISDN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Recurso Residencial Pospago NoLove. Login_CLU por MSISDN. </t>
-  </si>
-  <si>
-    <t>Recurso Empresa Pospago Love. Login_CLU por CIF.</t>
-  </si>
-  <si>
-    <t>Residencial Pospago NoLove</t>
-  </si>
-  <si>
-    <t>Residencial Pospago Love</t>
-  </si>
-  <si>
-    <t>Empresa Pospago Love</t>
-  </si>
-  <si>
-    <t>Prepago</t>
-  </si>
-  <si>
     <t>beta1234</t>
   </si>
   <si>
-    <t>43515511V</t>
+    <t>635656921</t>
+  </si>
+  <si>
+    <t>Mercado</t>
+  </si>
+  <si>
+    <t>Residencial Pospago</t>
+  </si>
+  <si>
+    <t>Empresa Pospago</t>
+  </si>
+  <si>
+    <t>Cliente Love</t>
+  </si>
+  <si>
+    <t>Residencial Prepago</t>
+  </si>
+  <si>
+    <t>Cliente No Love</t>
+  </si>
+  <si>
+    <t>Cliente No Love. Acceso MiLinea OK</t>
+  </si>
+  <si>
+    <t>Cliente No Love. Acceso Facturas OK</t>
+  </si>
+  <si>
+    <t>Cliente No Love. Acceso Dashboard OK.Sin CPs</t>
+  </si>
+  <si>
+    <t>Cliente No Love. Acceso Dashboard OK.Con CPs</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cliente NoLove. Login_CLU por MSISDN. </t>
+  </si>
+  <si>
+    <t>Cliente Love. Login_CLU por CIF.</t>
+  </si>
+  <si>
+    <t>Cliente No Love. Login_CLU por MSISDN</t>
+  </si>
+  <si>
+    <t>Cliente No Love. Acceso mi contrato OK</t>
   </si>
 </sst>
 </file>
@@ -517,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -537,7 +558,7 @@
         <v>655758100</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -545,60 +566,84 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="7" t="s">
+    <row r="3" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="23" t="s">
-        <v>10</v>
+    <row r="4" spans="1:2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="24" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="24" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="3">
+    <row r="8" spans="1:2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="3">
         <v>615761875</v>
       </c>
     </row>
-    <row r="8" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="5">
+    <row r="10" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="5">
         <v>11223344</v>
       </c>
     </row>
-    <row r="9" spans="1:2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>12</v>
+    <row r="11" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -609,10 +654,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -627,7 +672,7 @@
       </c>
       <c r="B1" s="9"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>2</v>
       </c>
@@ -635,81 +680,113 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="7" t="s">
+    <row r="3" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="12">
+    <row r="5" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="12">
         <v>655758100</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="14"/>
-    </row>
-    <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="16" t="s">
+    <row r="6" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="14"/>
+    </row>
+    <row r="7" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="16" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="17">
+    <row r="9" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="17">
         <v>655758200</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="17" t="s">
+    <row r="10" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="17" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="17" t="s">
+    <row r="11" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="17" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="12">
+    <row r="13" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="12">
         <v>655758100</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="14">
+    <row r="14" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="14">
         <v>123456</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="16" t="s">
+    <row r="15" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="16" t="s">
         <v>5</v>
       </c>
     </row>
@@ -720,10 +797,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:B6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -748,45 +825,61 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="3">
-        <v>635656921</v>
+    <row r="3" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="5">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3">
+        <v>635656921</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="5">
         <v>44332211</v>
       </c>
     </row>
-    <row r="6" spans="1:2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
     <row r="9" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -795,10 +888,174 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B42"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="18">
+        <v>655758100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="18">
+        <v>655758100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="5">
+        <v>44332211</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B57"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -811,188 +1068,188 @@
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3">
-        <v>615761875</v>
+      <c r="B1" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5">
-        <v>11223344</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="23">
-        <v>655758100</v>
+        <v>12</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="23">
+        <v>635649220</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="24">
+        <v>44332211</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="3">
+        <v>615761875</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="5">
+        <v>11223344</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="23">
+        <v>655758100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="24" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="25" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="3">
+    <row r="15" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="25" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="3">
         <v>635656921</v>
       </c>
     </row>
-    <row r="8" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="5">
+    <row r="18" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="5">
         <v>44332211</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="23">
-        <v>691852789</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="24">
-        <v>4603026</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="25" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" s="3">
-        <v>653318896</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" s="5">
-        <v>87654321</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="23">
-        <v>635658486</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17" s="24" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" s="25" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B19" s="3">
-        <v>635658400</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B20" s="5">
-        <v>123456</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>16</v>
+        <v>4</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="23">
+        <v>691852789</v>
       </c>
     </row>
     <row r="22" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="B22" s="23" t="s">
-        <v>20</v>
+        <v>2</v>
+      </c>
+      <c r="B22" s="24">
+        <v>4603026</v>
       </c>
     </row>
     <row r="23" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="B23" s="24">
-        <v>37560000</v>
+        <v>12</v>
+      </c>
+      <c r="B23" s="24" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="26" t="s">
+      <c r="A24" s="22" t="s">
         <v>4</v>
       </c>
       <c r="B24" s="25" t="s">
@@ -1003,62 +1260,117 @@
       <c r="A25" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>10</v>
+      <c r="B25" s="3">
+        <v>653318896</v>
       </c>
     </row>
     <row r="26" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B26" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="5">
+        <v>87654321</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B27" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="7" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="B28" s="23">
-        <v>635649220</v>
       </c>
     </row>
     <row r="29" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="B29" s="24">
-        <v>44332211</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="B30" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" s="23">
+        <v>635658486</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B30" s="24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="22"/>
+      <c r="B31" s="24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" s="25" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="33" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="34" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="35" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="36" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="33" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" s="3">
+        <v>635658400</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B34" s="5">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
     <row r="37" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="38" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="39" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="40" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="41" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="42" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="49" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="50" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="51" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="52" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="53" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="54" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="55" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="56" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="57" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>